<commit_message>
Bug fix in excel progressive numbers
</commit_message>
<xml_diff>
--- a/static-data/masks/GoT/discharges_GoT.xlsx
+++ b/static-data/masks/GoT/discharges_GoT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbolzon/Documents/workspace/MITgcm_BC_IC/static-data/masks/GoT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2C62A9-ED1E-9C4F-AA77-3741F6CE0E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69579797-9523-1B40-A479-CA8B3C7F0E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="5520" windowWidth="33940" windowHeight="15440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3040" yWindow="8320" windowWidth="33940" windowHeight="15440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="river_locations" sheetId="1" r:id="rId1"/>
@@ -974,19 +974,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="discharges_1" connectionId="1" xr16:uid="{C4A2FD47-A870-404C-93B3-16CB96E1512D}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="NADRI_OPER_1_1" connectionId="4" xr16:uid="{C52A1C6E-68E4-6C4E-95B7-EBFF5C9FAA26}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="NADRI_OPER_1_1" connectionId="4" xr16:uid="{C52A1C6E-68E4-6C4E-95B7-EBFF5C9FAA26}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="NADRI_OPER_1" connectionId="3" xr16:uid="{374F9F88-D389-C748-933E-5A161082CD25}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="NADRI_OPER_1" connectionId="3" xr16:uid="{374F9F88-D389-C748-933E-5A161082CD25}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="GoT_OPER" connectionId="2" xr16:uid="{00000000-0016-0000-0000-000001000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="GoT_OPER" connectionId="2" xr16:uid="{00000000-0016-0000-0000-000001000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="discharges_1" connectionId="1" xr16:uid="{C4A2FD47-A870-404C-93B3-16CB96E1512D}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1314,7 +1314,7 @@
   <dimension ref="B1:BI8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1683,7 +1683,7 @@
     </row>
     <row r="4" spans="2:61" x14ac:dyDescent="0.2">
       <c r="B4" s="18">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>14</v>
@@ -1865,7 +1865,7 @@
     </row>
     <row r="5" spans="2:61" x14ac:dyDescent="0.2">
       <c r="B5" s="18">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>15</v>
@@ -2047,7 +2047,7 @@
     </row>
     <row r="6" spans="2:61" x14ac:dyDescent="0.2">
       <c r="B6" s="18">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>2</v>
@@ -2229,7 +2229,7 @@
     </row>
     <row r="7" spans="2:61" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="18">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>7</v>

</xml_diff>